<commit_message>
- Create EditPage - Implement method for editing transaction and write to .xlsx - Add new JUnit Test and UAT
</commit_message>
<xml_diff>
--- a/expense-income.xlsx
+++ b/expense-income.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -30,25 +30,22 @@
     <t>amount</t>
   </si>
   <si>
+    <t>EXPENSE</t>
+  </si>
+  <si>
+    <t>eating lunch</t>
+  </si>
+  <si>
     <t>INCOME</t>
   </si>
   <si>
-    <t>เงินเดือนจากที่รัก</t>
+    <t>salary</t>
   </si>
   <si>
-    <t>เงินเดือนจากคุณแม่</t>
+    <t>first salary</t>
   </si>
   <si>
-    <t>EXPENSE</t>
-  </si>
-  <si>
-    <t>กินสเต็ก 52</t>
-  </si>
-  <si>
-    <t>เก็บเงินได้</t>
-  </si>
-  <si>
-    <t>ค่าปากกา</t>
+    <t>eating lunch in the morning</t>
   </si>
 </sst>
 </file>
@@ -102,7 +99,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -127,36 +124,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>43360.863452129626</v>
+        <v>43363.0</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>20.0</v>
+        <v>25000.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>43360.86368052083</v>
+        <v>43363.0</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>10.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="4">
@@ -164,16 +161,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>43360.99709289352</v>
+        <v>43363.0</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>99.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="5">
@@ -181,33 +178,16 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>43360.997855497684</v>
+        <v>43363.0</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" t="n">
-        <v>500.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>43360.99806297454</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="n">
-        <v>65.0</v>
+        <v>20000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>